<commit_message>
changed shfitish to ngrams, revamped arcane ngrams, added dash toggle to sniping, arcane ellipsis
</commit_message>
<xml_diff>
--- a/symbols.xlsx
+++ b/symbols.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\coding\bkqmk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B361428-8179-4BEE-A720-7701F4CBDDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6B8AEB-CCF8-49FB-A7C9-ADBE1E898107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25305" yWindow="5400" windowWidth="25200" windowHeight="9900" xr2:uid="{6365E638-7F9A-4BD8-BE60-7A40F09E580C}"/>
+    <workbookView minimized="1" xWindow="67590" yWindow="6180" windowWidth="18810" windowHeight="11385" xr2:uid="{6365E638-7F9A-4BD8-BE60-7A40F09E580C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="117">
   <si>
     <t>base</t>
   </si>
@@ -43,9 +42,6 @@
     <t>shifted</t>
   </si>
   <si>
-    <t>key</t>
-  </si>
-  <si>
     <t>shiftishL</t>
   </si>
   <si>
@@ -386,6 +382,9 @@
   </si>
   <si>
     <t>(?&lt;!)</t>
+  </si>
+  <si>
+    <t>'''''</t>
   </si>
 </sst>
 </file>
@@ -753,9 +752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435EBEB0-AA58-4716-AC03-B281A95CEDF4}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -777,8 +776,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" t="s">
-        <v>2</v>
+      <c r="A1" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -787,402 +786,405 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="E5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" t="s">
         <v>101</v>
       </c>
-      <c r="F5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" t="s">
-        <v>102</v>
-      </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="M5" t="s">
         <v>82</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J9" t="s">
+        <v>114</v>
+      </c>
+      <c r="L9" t="s">
         <v>115</v>
-      </c>
-      <c r="L9" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" t="s">
         <v>47</v>
       </c>
-      <c r="D12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J12" t="s">
-        <v>48</v>
-      </c>
       <c r="K12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L13" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="B15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:12">
       <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
+      <c r="L17" t="s">
         <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>106</v>
-      </c>
-      <c r="L17" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" spans="2:12">
       <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J18" t="s">
         <v>72</v>
-      </c>
-      <c r="C18" t="s">
-        <v>107</v>
-      </c>
-      <c r="J18" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:12">
       <c r="B20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
full symbol layers rework
</commit_message>
<xml_diff>
--- a/symbols.xlsx
+++ b/symbols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\coding\bkqmk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uranus\coding\bkqmk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6B8AEB-CCF8-49FB-A7C9-ADBE1E898107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E17FF6E-AA11-4301-97A4-3074FE204B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="67590" yWindow="6180" windowWidth="18810" windowHeight="11385" xr2:uid="{6365E638-7F9A-4BD8-BE60-7A40F09E580C}"/>
+    <workbookView xWindow="-19320" yWindow="-15" windowWidth="19440" windowHeight="12135" xr2:uid="{6365E638-7F9A-4BD8-BE60-7A40F09E580C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="123">
   <si>
     <t>base</t>
   </si>
@@ -93,21 +93,12 @@
     <t>_</t>
   </si>
   <si>
-    <t>shiftishB</t>
-  </si>
-  <si>
-    <t>shifted shiftishB</t>
-  </si>
-  <si>
     <t>!</t>
   </si>
   <si>
     <t>?</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>`</t>
   </si>
   <si>
@@ -135,9 +126,6 @@
     <t>RB_INDX</t>
   </si>
   <si>
-    <t>RB_INNR</t>
-  </si>
-  <si>
     <t>LB_INNR</t>
   </si>
   <si>
@@ -147,9 +135,6 @@
     <t>LH_INNR</t>
   </si>
   <si>
-    <t>RH_INNR</t>
-  </si>
-  <si>
     <t>TH_OUTR</t>
   </si>
   <si>
@@ -162,9 +147,6 @@
     <t>LT_INNR</t>
   </si>
   <si>
-    <t>RT_INNR</t>
-  </si>
-  <si>
     <t>spc</t>
   </si>
   <si>
@@ -183,18 +165,12 @@
     <t>;\n</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
     <t>s</t>
   </si>
   <si>
-    <t>@</t>
-  </si>
-  <si>
     <t>.com</t>
   </si>
   <si>
@@ -246,39 +222,21 @@
     <t>~</t>
   </si>
   <si>
-    <t>skipgram</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
-    <t>.gov</t>
-  </si>
-  <si>
     <t>||</t>
   </si>
   <si>
-    <t>++</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
     <t>-&gt;</t>
   </si>
   <si>
-    <t>v</t>
-  </si>
-  <si>
     <t>!=</t>
   </si>
   <si>
     <t>&lt;=</t>
   </si>
   <si>
-    <t>expand</t>
-  </si>
-  <si>
     <t>!==</t>
   </si>
   <si>
@@ -342,9 +300,6 @@
     <t>&gt;==</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -357,9 +312,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -384,14 +336,80 @@
     <t>(?&lt;!)</t>
   </si>
   <si>
-    <t>'''''</t>
+    <t>altishB</t>
+  </si>
+  <si>
+    <t>shifted altishB</t>
+  </si>
+  <si>
+    <t>wh</t>
+  </si>
+  <si>
+    <t>Wh</t>
+  </si>
+  <si>
+    <t>LH_INDX</t>
+  </si>
+  <si>
+    <t>LH_MDLE</t>
+  </si>
+  <si>
+    <t>LH_RING</t>
+  </si>
+  <si>
+    <t>LH_PNKY</t>
+  </si>
+  <si>
+    <t>LT_INDX</t>
+  </si>
+  <si>
+    <t>LT_RING</t>
+  </si>
+  <si>
+    <t>LT_MDLE</t>
+  </si>
+  <si>
+    <t>LT_PNKY</t>
+  </si>
+  <si>
+    <t>LB_INDX</t>
+  </si>
+  <si>
+    <t>LB_MDLE</t>
+  </si>
+  <si>
+    <t>LB_RING</t>
+  </si>
+  <si>
+    <t>LB_PNKY</t>
+  </si>
+  <si>
+    <t>LT_OUTR</t>
+  </si>
+  <si>
+    <t>LH_OUTR</t>
+  </si>
+  <si>
+    <t>LB_OUTR</t>
+  </si>
+  <si>
+    <t>`@gmail.com</t>
+  </si>
+  <si>
+    <t>`@live.com</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,13 +427,25 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -427,16 +457,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -454,9 +487,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -494,7 +527,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -600,7 +633,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -742,7 +775,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -750,11 +783,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435EBEB0-AA58-4716-AC03-B281A95CEDF4}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -765,20 +798,16 @@
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -795,403 +824,515 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="M1" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L2" t="s">
-        <v>92</v>
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" t="s">
-        <v>96</v>
+      <c r="I3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>42</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>79</v>
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" t="s">
-        <v>101</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" t="s">
-        <v>111</v>
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" t="s">
-        <v>69</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" t="s">
-        <v>93</v>
-      </c>
-      <c r="J9" t="s">
-        <v>114</v>
-      </c>
-      <c r="L9" t="s">
-        <v>115</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" t="s">
-        <v>88</v>
-      </c>
-      <c r="H10" t="s">
-        <v>94</v>
-      </c>
-      <c r="J10" t="s">
-        <v>113</v>
-      </c>
-      <c r="L10" t="s">
-        <v>112</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" t="s">
-        <v>70</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" t="s">
-        <v>47</v>
-      </c>
-      <c r="K12" t="s">
-        <v>91</v>
-      </c>
-      <c r="L12" t="s">
-        <v>68</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
+      <c r="I16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" t="s">
+        <v>122</v>
+      </c>
+      <c r="H28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="B29" t="s">
         <v>43</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="J29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="H32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="J33" t="s">
         <v>60</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" t="s">
-        <v>57</v>
-      </c>
-      <c r="L13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="B14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" t="s">
-        <v>102</v>
-      </c>
-      <c r="L14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>103</v>
-      </c>
-      <c r="L15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" t="s">
-        <v>104</v>
-      </c>
-      <c r="L16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12">
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" t="s">
-        <v>105</v>
-      </c>
-      <c r="L17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12">
-      <c r="B18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" t="s">
-        <v>106</v>
-      </c>
-      <c r="J18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12">
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" t="s">
-        <v>107</v>
-      </c>
-      <c r="L19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12">
-      <c r="B20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{09129AE1-6E4B-4696-877D-2752A961E620}"/>
+    <hyperlink ref="I18" r:id="rId1" xr:uid="{ED6A16C4-897F-4DE4-9940-8010518E73A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added ` shift to *
</commit_message>
<xml_diff>
--- a/symbols.xlsx
+++ b/symbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uranus\coding\bkqmk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E17FF6E-AA11-4301-97A4-3074FE204B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876D500D-C897-4E6D-81FB-D6564965583D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-15" windowWidth="19440" windowHeight="12135" xr2:uid="{6365E638-7F9A-4BD8-BE60-7A40F09E580C}"/>
   </bookViews>
@@ -787,7 +787,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>